<commit_message>
Add metadata 'unit' to datasets
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfm12099\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\KY5DTA9K\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\economia\Publicaciones\Indicadores_COVID19\envio_informatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Indicadores</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Afiliados</t>
   </si>
   <si>
-    <t>Fuente: ICANE a partir de Afiliaciones a la Seguridad Social de la Tesorería General de la Seguridad Social</t>
-  </si>
-  <si>
     <t>Afiliados asalariados</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
     <t>Índice de comercio al por menor</t>
   </si>
   <si>
+    <t>Tráfico aéreo</t>
+  </si>
+  <si>
     <t>Tráfico del puerto</t>
   </si>
   <si>
@@ -230,7 +230,16 @@
     <t>Fuente: ICANE a partir de Estadística de tráfico aéreo de AENA</t>
   </si>
   <si>
-    <t>Tráfico aéreo de pasajeros</t>
+    <t>Afiliados (a último día de mes)</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Afiliaciones a la Seguridad Social a último día de mes de la Tesorería General de la Seguridad Social</t>
+  </si>
+  <si>
+    <t>Toneladas</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Consumo de Productos Pretrolíferos del CORES</t>
   </si>
 </sst>
 </file>
@@ -619,14 +628,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="102.5703125" style="10" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="10"/>
@@ -799,46 +808,46 @@
         <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -846,7 +855,7 @@
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -854,21 +863,21 @@
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -876,23 +885,29 @@
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -900,21 +915,21 @@
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -922,7 +937,7 @@
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -930,7 +945,7 @@
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -938,7 +953,7 @@
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>66</v>
@@ -1148,7 +1163,7 @@
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>

</xml_diff>

<commit_message>
Add annual data file
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t>Indicadores</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Deuda sobre el PIB</t>
   </si>
   <si>
-    <t>Empresas y establecimientos</t>
-  </si>
-  <si>
     <t>Ìndice de confianza empresarial</t>
   </si>
   <si>
@@ -240,13 +237,49 @@
   </si>
   <si>
     <t>Fuente: ICANE a partir de Consumo de Productos Pretrolíferos del CORES</t>
+  </si>
+  <si>
+    <t>PIB. Precios corrientes</t>
+  </si>
+  <si>
+    <t>Miles de euros</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Contabilidad Regional de España Base 2015 del INE</t>
+  </si>
+  <si>
+    <t>PIB per cápita</t>
+  </si>
+  <si>
+    <t>Euros</t>
+  </si>
+  <si>
+    <t>Sanidad</t>
+  </si>
+  <si>
+    <t>Gasto sanitario público consolidado. Sector CC.AA</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Estadística de Gasto sanitario público del Ministerio de Sanidad</t>
+  </si>
+  <si>
+    <t>Gasto sanitario público consolidado per cápita. Sector CC.AA</t>
+  </si>
+  <si>
+    <t>Gasto sanitario público consolidado sobre el PIB. Sector CC.AA</t>
+  </si>
+  <si>
+    <t>Los datos de 2017 y 2018 son provisionales</t>
+  </si>
+  <si>
+    <t>Los datos de 2017 son provisionales y 2018 son avance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +309,19 @@
       <color rgb="FFFF0000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -319,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,13 +385,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,563 +673,687 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.5703125" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="50" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="102.5703125" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>4</v>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>56</v>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>57</v>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change in annual data export
Remove trend data
Export the whole serie
Add metadata JSON file
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
   <si>
     <t>Indicadores</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Deficit público sobre el PIB</t>
   </si>
   <si>
-    <t>Recaudación tributaria</t>
-  </si>
-  <si>
     <t>Empresas</t>
   </si>
   <si>
@@ -143,18 +140,12 @@
     <t>Indicador de actividad del sector servicios</t>
   </si>
   <si>
-    <t>Índice de comercio al por menor</t>
-  </si>
-  <si>
     <t>Tráfico aéreo</t>
   </si>
   <si>
     <t>Tráfico del puerto</t>
   </si>
   <si>
-    <t>Coyuntura turística hotelera</t>
-  </si>
-  <si>
     <t>Encuesta de ocupación turística extrahotelera</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>Nivel calidad y condiciones de vida</t>
   </si>
   <si>
-    <t>IPC</t>
-  </si>
-  <si>
     <t>Índice</t>
   </si>
   <si>
@@ -269,10 +257,43 @@
     <t>Gasto sanitario público consolidado sobre el PIB. Sector CC.AA</t>
   </si>
   <si>
-    <t>Los datos de 2017 y 2018 son provisionales</t>
-  </si>
-  <si>
-    <t>Los datos de 2017 son provisionales y 2018 son avance</t>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Los datos de 2017 son provisionales  2018 son avance</t>
+  </si>
+  <si>
+    <t>PIB. Índices de volumen</t>
+  </si>
+  <si>
+    <t>Ingresos tributarios netos anuales</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Informes de Recaudación Tributaria de la AEAT</t>
+  </si>
+  <si>
+    <t>Ingresos tributarios netos mensuales</t>
+  </si>
+  <si>
+    <t>Para una mejor interpretación la tasa de variación se da en términos absolutos al tratarse de un saldo de porcentaje</t>
+  </si>
+  <si>
+    <t>Índice de comercio al por menor a precios constantes</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Índice de Comercio al por Menor del INE</t>
+  </si>
+  <si>
+    <t>Pernoctaciones hoteleras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pernoctaciones </t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Coyuntura Turística Hotelera del INE</t>
+  </si>
+  <si>
+    <t>Índice de precios al consumo</t>
   </si>
 </sst>
 </file>
@@ -386,13 +407,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,42 +694,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="102.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="93.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -719,60 +743,60 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>82</v>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -781,7 +805,7 @@
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -815,96 +839,108 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="B16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -912,101 +948,101 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="B23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="B24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1015,7 +1051,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1024,16 +1060,16 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1041,41 +1077,43 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="B33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1083,125 +1121,137 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="B38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="5" t="s">
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+    <row r="43" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+    <row r="45" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1210,7 +1260,7 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1219,7 +1269,7 @@
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1227,26 +1277,26 @@
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1255,7 +1305,7 @@
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1264,7 +1314,7 @@
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1272,80 +1322,91 @@
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
+      <c r="B60" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Change variable names on quarterly datasets
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
   <si>
     <t>Indicadores</t>
   </si>
@@ -258,13 +258,19 @@
   </si>
   <si>
     <t>Gasto sanitario público consolidado sobre el PIB sector CC.AA</t>
+  </si>
+  <si>
+    <t>Para una mejor interpretación la tasa de variación se da en términos absolutos al tratarse de una tasa</t>
+  </si>
+  <si>
+    <t>Tasa de empleo EPA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +302,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -339,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,6 +368,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,70 +706,70 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -833,64 +851,64 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -902,83 +920,83 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1025,11 +1043,13 @@
       <c r="D25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="26" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>69</v>
@@ -1040,186 +1060,205 @@
       <c r="D26" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="C29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E29" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="C30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="C32" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E32" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="7" t="s">
+      <c r="C33" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="7" t="s">
+      <c r="C34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="C36" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="C38" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E38" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="C39" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E39" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="B40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E40" s="7" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add datasets of 'Sector Exterior'
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="125">
   <si>
     <t>Economía</t>
   </si>
@@ -356,14 +356,56 @@
     <t>Sociedades mercantiles disueltas</t>
   </si>
   <si>
-    <t>Los datos son provisionales desde el año 2019</t>
+    <t>Indicadores</t>
+  </si>
+  <si>
+    <t>Unidades primeras tablas</t>
+  </si>
+  <si>
+    <t>Unidades segundas tablas</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Notas especiales para las visiones globales</t>
+  </si>
+  <si>
+    <t>Los datos son provisionales desde enero de 2019</t>
+  </si>
+  <si>
+    <t>Sector exterior</t>
+  </si>
+  <si>
+    <t>Importaciones</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Estadisitca de Comercio Exterior de la AEAT</t>
+  </si>
+  <si>
+    <t>Los datos son provisionales desde enero 2019</t>
+  </si>
+  <si>
+    <t>Exportaciones</t>
+  </si>
+  <si>
+    <t>Saldo comercial</t>
+  </si>
+  <si>
+    <t>Tasa de cobertura</t>
+  </si>
+  <si>
+    <t>Los datos son provisionales desde enero 2019. Para una mejor interpretación la tasa de variación se da en términos absolutos al tratarse de una tasa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,8 +449,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +467,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,19 +504,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -470,6 +520,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,872 +811,990 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="145.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="111.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="50" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="145.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="111.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
+      <c r="B11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="B12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="C14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="C16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="C19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E26" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="C29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B30" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="C30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="9" t="s">
+      <c r="C31" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E31" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="C32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B34" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="9" t="s">
+      <c r="C34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="C35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B36" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="9" t="s">
+      <c r="C36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B37" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="C37" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B39" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="C39" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B40" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="9" t="s">
+      <c r="C40" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="E40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="C41" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E41" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B42" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="C42" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E42" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="C43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E43" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="9" t="s">
+      <c r="C44" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E44" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B45" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="9" t="s">
+      <c r="C45" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E45" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B46" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="9" t="s">
+      <c r="C46" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E46" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B48" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" s="9" t="s">
+      <c r="C48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B49" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" s="9" t="s">
+      <c r="C49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E49" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B50" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="9" t="s">
+      <c r="C50" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E50" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B52" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="9" t="s">
+      <c r="C52" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B53" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="9" t="s">
+      <c r="C53" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E53" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
+      <c r="B54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E54" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F54" s="6" t="s">
         <v>89</v>
       </c>
     </row>
+    <row r="55" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add monthly and quarterly widgets
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="145">
   <si>
     <t>Economía</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Fuente: ICANE a partir de Informes Anuales de Recaudación Tributaria de la AEAT</t>
   </si>
   <si>
-    <t>Los datos de 2018 son provisionales y los de 2019 y 2020 avance</t>
-  </si>
-  <si>
     <t>Fuente: ICANE a partir de Informes Mensuales de Recaudación Tributaria de la AEAT</t>
   </si>
   <si>
@@ -438,6 +435,30 @@
   </si>
   <si>
     <t>Los datos de mayo del año 2019 y posteriores son provisionales</t>
+  </si>
+  <si>
+    <t>Gasto en productos farmacéuticos y sanitarios</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Gasto en productos farmacéuticos y sanitarios de Ministeriro de Hacienda</t>
+  </si>
+  <si>
+    <t>Gasto devengado neto acumulado anual. Cantabria está realizando la revisión de la información de toda la serie para homogeneizar los criterios aplicados en la extracción de la información, por lo que las tres partidas de gasto pueden presentar modificaciones en próximas publicaciones.</t>
+  </si>
+  <si>
+    <t>Transporte de mercancías por carretera</t>
+  </si>
+  <si>
+    <t>Miles de de toneladas</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Transporte de Mercacias por Carretera del Ministerio de Transporte, Movilidad y Agenda Urbana</t>
+  </si>
+  <si>
+    <t>Los datos de 2018 son provisionales y los de 2019 avance</t>
+  </si>
+  <si>
+    <t>Datos acumulados a final de periodo. Los datos de 2018 son provisionales y los de 2019 y 2020 avance</t>
   </si>
 </sst>
 </file>
@@ -489,7 +510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,12 +520,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,16 +567,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,32 +873,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -959,7 +966,7 @@
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>27</v>
@@ -1003,7 +1010,7 @@
         <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -1018,14 +1025,14 @@
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>2</v>
@@ -1035,15 +1042,15 @@
         <v>42</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>2</v>
@@ -1053,41 +1060,43 @@
         <v>45</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>1</v>
@@ -1103,7 +1112,7 @@
     </row>
     <row r="16" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>1</v>
@@ -1119,124 +1128,124 @@
     </row>
     <row r="17" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>2</v>
@@ -1249,25 +1258,23 @@
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>9</v>
@@ -1285,7 +1292,7 @@
     </row>
     <row r="27" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>9</v>
@@ -1303,23 +1310,25 @@
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>51</v>
@@ -1335,10 +1344,10 @@
     </row>
     <row r="30" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>2</v>
@@ -1346,14 +1355,12 @@
       <c r="D30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>55</v>
@@ -1371,7 +1378,7 @@
     </row>
     <row r="32" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>55</v>
@@ -1387,245 +1394,245 @@
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="E34" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+    <row r="40" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="C41" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="C44" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B45" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="13" t="s">
+      <c r="C45" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-    </row>
-    <row r="45" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>115</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>35</v>
@@ -1634,160 +1641,168 @@
         <v>2</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="C53" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="C56" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="C57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="E57" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>27</v>
@@ -1796,130 +1811,176 @@
         <v>2</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="D60" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F60" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="15" t="s">
+      <c r="B65" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="E65" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E62" s="10" t="s">
+      <c r="C66" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F62" s="10"/>
-    </row>
-    <row r="63" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="10"/>
-    </row>
-    <row r="64" spans="1:6" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F64" s="10"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F65" s="10"/>
+      <c r="F68" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Quarterly updates + 2 new datasets
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="151">
   <si>
     <t>Economía</t>
   </si>
@@ -542,7 +542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -565,11 +565,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,6 +600,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -873,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:A71"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,51 +1114,49 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
+      <c r="A15" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>1</v>
@@ -1162,173 +1172,169 @@
     </row>
     <row r="18" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>93</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>9</v>
@@ -1346,42 +1352,46 @@
     </row>
     <row r="29" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>2</v>
@@ -1389,17 +1399,15 @@
       <c r="D31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>2</v>
@@ -1407,14 +1415,12 @@
       <c r="D32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>55</v>
@@ -1431,176 +1437,180 @@
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>131</v>
+      <c r="A34" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+    <row r="35" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="6"/>
+        <v>132</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="6"/>
+    <row r="37" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+    <row r="42" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+    <row r="44" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>21</v>
@@ -1609,14 +1619,14 @@
         <v>2</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>21</v>
@@ -1625,77 +1635,73 @@
         <v>2</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>112</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>134</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>134</v>
@@ -1704,151 +1710,159 @@
     </row>
     <row r="51" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="C54" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="6" t="s">
+      <c r="C55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E55" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="11" t="s">
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B56" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="9" t="s">
+      <c r="C56" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E56" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D56" s="6" t="s">
+      <c r="C58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="C59" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E59" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>27</v>
@@ -1857,80 +1871,80 @@
         <v>2</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="D62" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="6" t="s">
-        <v>85</v>
-      </c>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+    <row r="64" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>27</v>
@@ -1939,34 +1953,26 @@
         <v>2</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F66" s="6"/>
+    <row r="66" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>27</v>
@@ -1984,10 +1990,10 @@
     </row>
     <row r="68" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>2</v>
@@ -1996,53 +2002,89 @@
         <v>115</v>
       </c>
       <c r="E68" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="11" t="s">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B72" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" s="9" t="s">
+      <c r="C72" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-    </row>
-    <row r="71" spans="1:6" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B73" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" s="9" t="s">
+      <c r="C73" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E73" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F71" s="9"/>
+      <c r="F73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
New dataset: 'Tasa de apertura'
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="162">
   <si>
     <t>Economía</t>
   </si>
@@ -501,6 +501,15 @@
   </si>
   <si>
     <t>Fuente: ICANE a partir de Contabilidad Trimestral de España del INE y Contabilidad Trimestral de Cantabria Base 2015 del ICANE</t>
+  </si>
+  <si>
+    <t>Tasa de apertura</t>
+  </si>
+  <si>
+    <t>Fuente: ICANE a partir de Estadisitca de Comercio Exterior de la AEAT, Contabilidad Nacional Trimestral de España del INE y Contabilidad Trimestral de Cantabria Base 2015 del ICANE</t>
+  </si>
+  <si>
+    <t>Tasa de apertura= (saldo comercial/PIB)*100. Para una mejor interpretación la tasa de variación se da en términos absolutos al tratarse de un saldo de porcentajes. Datos provisionales</t>
   </si>
 </sst>
 </file>
@@ -901,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:E54"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,19 +1002,19 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1849,37 +1858,37 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="10" t="s">
+      <c r="C58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="6" t="s">
         <v>93</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="10" t="s">
+      <c r="C59" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="6" t="s">
         <v>93</v>
       </c>
       <c r="F59" s="6"/>
@@ -2110,49 +2119,65 @@
       </c>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B77" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="C77" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E77" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F76" s="6"/>
+      <c r="F77" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Change notes of quarterly series
</commit_message>
<xml_diff>
--- a/docs/Fuentes y unidades.xlsx
+++ b/docs/Fuentes y unidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="164">
   <si>
     <t>Economía</t>
   </si>
@@ -509,7 +509,13 @@
     <t>Fuente: ICANE a partir de Estadisitca de Comercio Exterior de la AEAT, Contabilidad Nacional Trimestral de España del INE y Contabilidad Trimestral de Cantabria Base 2015 del ICANE</t>
   </si>
   <si>
-    <t>Tasa de apertura= (saldo comercial/PIB)*100. Para una mejor interpretación la tasa de variación se da en términos absolutos al tratarse de un saldo de porcentajes. Datos provisionales</t>
+    <t>Los datos del primer trimestre del año 2019 y posteriores son provisionales.</t>
+  </si>
+  <si>
+    <t>Para una mejor interpretación es el dato del indicador y no su tasa de variación anual</t>
+  </si>
+  <si>
+    <t>Tasa de apertura= (saldo comercial/PIB)*100.  Para una mejor interpretación es el dato del indicador y no su tasa de variación anual</t>
   </si>
 </sst>
 </file>
@@ -912,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,9 +927,9 @@
     <col min="1" max="1" width="50" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="145.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="111.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="4" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
@@ -1182,7 +1188,9 @@
       <c r="D16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>162</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1800,8 +1808,8 @@
       <c r="D54" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>149</v>
+      <c r="E54" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="F54" s="6"/>
     </row>
@@ -1871,7 +1879,7 @@
         <v>151</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="F58" s="6"/>
     </row>
@@ -1889,7 +1897,7 @@
         <v>151</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="F59" s="6"/>
     </row>
@@ -2131,7 +2139,7 @@
         <v>160</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F74" s="6"/>
     </row>

</xml_diff>